<commit_message>
developing univariate tables for mortality and Addison's + KM curve
</commit_message>
<xml_diff>
--- a/thabs_PHD/MV_mortality table.xlsx
+++ b/thabs_PHD/MV_mortality table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sempajb\Documents\GitHub\Contractual_wk\thabs_PHD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{624CC314-D1CA-4A7E-BE64-5C0B836E93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD5D0B6-24A0-46DF-B463-AE9DF66DA041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{B50FBFE2-7444-4A8A-B71B-373D504BC3D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B50FBFE2-7444-4A8A-B71B-373D504BC3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>term</t>
   </si>
@@ -85,6 +86,15 @@
   </si>
   <si>
     <t>Variables</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>ACTH</t>
+  </si>
+  <si>
+    <t>Stimulated_cortisol</t>
   </si>
 </sst>
 </file>
@@ -120,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEB78A6-F010-4A5F-B28A-E4DED6961795}">
-  <dimension ref="B2:K15"/>
+  <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:H15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,15 +533,15 @@
         <v>1.01039302</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H7" si="0">EXP(C4)</f>
+        <f>EXP(C4)</f>
         <v>1.3734812840567086</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:J7" si="1">EXP(E4)</f>
+        <f>EXP(E4)</f>
         <v>0.68681121001279966</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
+        <f>EXP(F4)</f>
         <v>2.7466803032048674</v>
       </c>
       <c r="K4">
@@ -554,15 +565,15 @@
         <v>0.10514490999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>EXP(C5)</f>
         <v>0.98330143286189686</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f>EXP(E5)</f>
         <v>0.87038117508832591</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
+        <f>EXP(F5)</f>
         <v>1.1108715750926703</v>
       </c>
       <c r="K5">
@@ -586,15 +597,15 @@
         <v>0.14224036000000001</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>EXP(C6)</f>
         <v>0.84592556320694101</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f>EXP(E6)</f>
         <v>0.62071193217995146</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
+        <f>EXP(F6)</f>
         <v>1.1528537151567797</v>
       </c>
       <c r="K6">
@@ -618,15 +629,15 @@
         <v>5.248879E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>EXP(C7)</f>
         <v>1.0220160743657043</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f>EXP(E7)</f>
         <v>0.99110544766497766</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
+        <f>EXP(F7)</f>
         <v>1.053890747897035</v>
       </c>
       <c r="K7">
@@ -735,7 +746,155 @@
         <v>0.159972</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>6.6815449200000003</v>
+      </c>
+      <c r="D21">
+        <v>3.6034752000000001E-3</v>
+      </c>
+      <c r="E21">
+        <v>2.3702713379999998</v>
+      </c>
+      <c r="F21">
+        <v>10.992818508999999</v>
+      </c>
+      <c r="H21">
+        <f>EXP(C21)</f>
+        <v>797.55031214641087</v>
+      </c>
+      <c r="I21">
+        <f>EXP(E21)</f>
+        <v>10.70029528696832</v>
+      </c>
+      <c r="J21">
+        <f>EXP(F21)</f>
+        <v>59445.696384857634</v>
+      </c>
+      <c r="K21">
+        <v>3.6034752000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>1.7788129999999999E-2</v>
+      </c>
+      <c r="D22">
+        <v>9.2376599700000006E-2</v>
+      </c>
+      <c r="E22">
+        <v>-3.1350039999999998E-3</v>
+      </c>
+      <c r="F22">
+        <v>3.8711267000000001E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:H23" si="0">EXP(C22)</f>
+        <v>1.0179472810504786</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I23" si="1">EXP(E22)</f>
+        <v>0.99686990499379502</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:J23" si="2">EXP(F22)</f>
+        <v>1.0394703109360717</v>
+      </c>
+      <c r="K22">
+        <v>9.2376599700000006E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>-1.7587829999999999E-2</v>
+      </c>
+      <c r="D23">
+        <v>1.082213E-4</v>
+      </c>
+      <c r="E23">
+        <v>-2.6013217000000002E-2</v>
+      </c>
+      <c r="F23">
+        <v>-9.1624380000000002E-3</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.98256593310924689</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0.97432221190697244</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0.99087940922997575</v>
+      </c>
+      <c r="K23">
+        <v>1.082213E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EEDAAD-2B5A-4B31-9275-73162A6ADD10}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>